<commit_message>
trying to get automatic department from requester and also fix form-control for status form
</commit_message>
<xml_diff>
--- a/updated_inventory_list_xls2.xlsx
+++ b/updated_inventory_list_xls2.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13710"/>
   </bookViews>
   <sheets>
-    <sheet name="updated_inventory_list (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="updated_inventory_list_xls2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -30,9 +30,6 @@
     <t>date_created</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>vendor_id</t>
   </si>
   <si>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sleeve : Well Plates </t>
+  </si>
+  <si>
+    <t>notes_inv</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1411,7 @@
   <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G2" sqref="G2:I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1419,7 @@
     <col min="1" max="1" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1444,42 +1444,42 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
         <v>13.85</v>
@@ -1487,37 +1487,25 @@
       <c r="C2" s="3">
         <v>43292</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
       <c r="F2" s="3">
         <v>43292</v>
       </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>32</v>
@@ -1525,37 +1513,25 @@
       <c r="C3" s="3">
         <v>43292</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
       <c r="F3" s="3">
         <v>43292</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>3.3</v>
@@ -1563,37 +1539,25 @@
       <c r="C4" s="3">
         <v>43292</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
       <c r="F4" s="3">
         <v>43292</v>
       </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
       <c r="J4" s="1">
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2">
         <v>14.5</v>
@@ -1601,37 +1565,25 @@
       <c r="C5" s="3">
         <v>43292</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
       <c r="F5" s="3">
         <v>43292</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
       <c r="J5" s="1">
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2">
         <v>3.3</v>
@@ -1639,37 +1591,25 @@
       <c r="C6" s="3">
         <v>43292</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
       <c r="F6" s="3">
         <v>43292</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
       <c r="J6" s="1">
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2">
         <v>27</v>
@@ -1677,37 +1617,25 @@
       <c r="C7" s="3">
         <v>43292</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
       <c r="F7" s="3">
         <v>43292</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2">
         <v>14</v>
@@ -1715,37 +1643,25 @@
       <c r="C8" s="3">
         <v>43292</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
       <c r="F8" s="3">
         <v>43292</v>
       </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="2">
         <v>11</v>
@@ -1753,37 +1669,25 @@
       <c r="C9" s="3">
         <v>43292</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
       <c r="F9" s="3">
         <v>43292</v>
       </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="2">
         <v>11</v>
@@ -1791,37 +1695,25 @@
       <c r="C10" s="3">
         <v>43292</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
       <c r="F10" s="3">
         <v>43292</v>
       </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2">
         <v>11</v>
@@ -1829,37 +1721,25 @@
       <c r="C11" s="3">
         <v>43292</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
       <c r="F11" s="3">
         <v>43292</v>
       </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1867,37 +1747,25 @@
       <c r="C12" s="3">
         <v>43292</v>
       </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
       <c r="F12" s="3">
         <v>43292</v>
       </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="2">
         <v>25.61</v>
@@ -1905,37 +1773,25 @@
       <c r="C13" s="3">
         <v>43292</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
       <c r="F13" s="3">
         <v>43292</v>
       </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
       <c r="J13" s="1">
         <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2">
         <v>11</v>
@@ -1943,37 +1799,25 @@
       <c r="C14" s="3">
         <v>43292</v>
       </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
       <c r="F14" s="3">
         <v>43292</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
       <c r="J14" s="1">
         <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
         <v>85.04</v>
@@ -1981,37 +1825,25 @@
       <c r="C15" s="3">
         <v>43292</v>
       </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
       <c r="F15" s="3">
         <v>43292</v>
       </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
       <c r="J15" s="1">
         <v>1</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <v>24</v>
@@ -2019,37 +1851,25 @@
       <c r="C16" s="3">
         <v>43292</v>
       </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
       <c r="F16" s="3">
         <v>43292</v>
       </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
       <c r="J16" s="1">
         <v>1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
         <v>31</v>
@@ -2057,37 +1877,25 @@
       <c r="C17" s="3">
         <v>43292</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
       <c r="F17" s="3">
         <v>43292</v>
       </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
       <c r="J17" s="1">
         <v>1</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2">
         <v>25</v>
@@ -2095,37 +1903,25 @@
       <c r="C18" s="3">
         <v>43292</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
       <c r="F18" s="3">
         <v>43292</v>
       </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
       <c r="J18" s="1">
         <v>1</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2">
         <v>19.25</v>
@@ -2133,81 +1929,57 @@
       <c r="C19" s="3">
         <v>43292</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
       <c r="F19" s="3">
         <v>43292</v>
       </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43292</v>
+      </c>
+      <c r="F20" s="3">
+        <v>43292</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>43292</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>43292</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="2">
         <v>9</v>
@@ -2215,40 +1987,28 @@
       <c r="C21" s="3">
         <v>43292</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
       <c r="F21" s="3">
         <v>43292</v>
       </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
       <c r="J21" s="1">
         <v>1</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="2">
         <v>11</v>
@@ -2256,37 +2016,25 @@
       <c r="C22" s="3">
         <v>43292</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
       <c r="F22" s="3">
         <v>43292</v>
       </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
       <c r="J22" s="1">
         <v>1</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B23" s="2">
         <v>50</v>
@@ -2294,37 +2042,25 @@
       <c r="C23" s="3">
         <v>43292</v>
       </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
       <c r="F23" s="3">
         <v>43292</v>
       </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
       <c r="J23" s="1">
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2">
         <v>14</v>
@@ -2332,37 +2068,25 @@
       <c r="C24" s="3">
         <v>43292</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
       <c r="F24" s="3">
         <v>43292</v>
       </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
       <c r="J24" s="1">
         <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2">
         <v>7</v>
@@ -2370,40 +2094,28 @@
       <c r="C25" s="3">
         <v>43292</v>
       </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
       <c r="F25" s="3">
         <v>43292</v>
       </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
       <c r="J25" s="1">
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2">
         <v>31</v>
@@ -2411,37 +2123,25 @@
       <c r="C26" s="3">
         <v>43292</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
       <c r="F26" s="3">
         <v>43292</v>
       </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
       <c r="J26" s="1">
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2">
         <v>24</v>
@@ -2449,37 +2149,25 @@
       <c r="C27" s="3">
         <v>43292</v>
       </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
       <c r="F27" s="3">
         <v>43292</v>
       </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
       <c r="J27" s="1">
         <v>1</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2">
         <v>20</v>
@@ -2487,37 +2175,25 @@
       <c r="C28" s="3">
         <v>43292</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
       <c r="F28" s="3">
         <v>43292</v>
       </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
       <c r="J28" s="1">
         <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="2">
         <v>17</v>
@@ -2525,37 +2201,25 @@
       <c r="C29" s="3">
         <v>43292</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
       <c r="F29" s="3">
         <v>43292</v>
       </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
       <c r="J29" s="1">
         <v>1</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="2">
         <v>39.75</v>
@@ -2563,37 +2227,25 @@
       <c r="C30" s="3">
         <v>43292</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
       <c r="F30" s="3">
         <v>43292</v>
       </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
       <c r="J30" s="1">
         <v>1</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2">
         <v>144</v>
@@ -2601,37 +2253,25 @@
       <c r="C31" s="3">
         <v>43292</v>
       </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
       <c r="F31" s="3">
         <v>43292</v>
       </c>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
       <c r="J31" s="1">
         <v>1</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="2">
         <v>72</v>
@@ -2639,37 +2279,25 @@
       <c r="C32" s="3">
         <v>43292</v>
       </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
       <c r="F32" s="3">
         <v>43292</v>
       </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
       <c r="J32" s="1">
         <v>1</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="2">
         <v>63</v>
@@ -2677,40 +2305,28 @@
       <c r="C33" s="3">
         <v>43292</v>
       </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
       <c r="F33" s="3">
         <v>43292</v>
       </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
       <c r="J33" s="1">
         <v>1</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" s="2">
         <v>35.75</v>
@@ -2718,37 +2334,25 @@
       <c r="C34" s="3">
         <v>43292</v>
       </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
       <c r="F34" s="3">
         <v>43292</v>
       </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
       <c r="J34" s="1">
         <v>1</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="2">
         <v>20.25</v>
@@ -2756,37 +2360,25 @@
       <c r="C35" s="3">
         <v>43292</v>
       </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
       <c r="F35" s="3">
         <v>43292</v>
       </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0</v>
-      </c>
       <c r="J35" s="1">
         <v>1</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="2">
         <v>28</v>
@@ -2794,37 +2386,25 @@
       <c r="C36" s="3">
         <v>43292</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
       <c r="F36" s="3">
         <v>43292</v>
       </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
       <c r="J36" s="1">
         <v>1</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37" s="2">
         <v>58</v>
@@ -2832,40 +2412,28 @@
       <c r="C37" s="3">
         <v>43292</v>
       </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
       <c r="F37" s="3">
         <v>43292</v>
       </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
       <c r="J37" s="1">
         <v>1</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="2">
         <v>53</v>
@@ -2873,37 +2441,25 @@
       <c r="C38" s="3">
         <v>43292</v>
       </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
       <c r="F38" s="3">
         <v>43292</v>
       </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
       <c r="J38" s="1">
         <v>1</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="2">
         <v>20</v>
@@ -2911,37 +2467,25 @@
       <c r="C39" s="3">
         <v>43292</v>
       </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
       <c r="F39" s="3">
         <v>43292</v>
       </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0</v>
-      </c>
       <c r="J39" s="1">
         <v>1</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="2">
         <v>63</v>
@@ -2949,37 +2493,25 @@
       <c r="C40" s="3">
         <v>43292</v>
       </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
       <c r="F40" s="3">
         <v>43292</v>
       </c>
-      <c r="G40" s="1">
-        <v>0</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0</v>
-      </c>
       <c r="J40" s="1">
         <v>1</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" s="2">
         <v>7</v>
@@ -2987,37 +2519,25 @@
       <c r="C41" s="3">
         <v>43292</v>
       </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
       <c r="F41" s="3">
         <v>43292</v>
       </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0</v>
-      </c>
-      <c r="I41" s="1">
-        <v>0</v>
-      </c>
       <c r="J41" s="1">
         <v>1</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="2">
         <v>24</v>
@@ -3025,37 +2545,25 @@
       <c r="C42" s="3">
         <v>43292</v>
       </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
       <c r="F42" s="3">
         <v>43292</v>
       </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0</v>
-      </c>
       <c r="J42" s="1">
         <v>1</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2">
         <v>14</v>
@@ -3063,37 +2571,25 @@
       <c r="C43" s="3">
         <v>43292</v>
       </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
       <c r="F43" s="3">
         <v>43292</v>
       </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0</v>
-      </c>
-      <c r="I43" s="1">
-        <v>0</v>
-      </c>
       <c r="J43" s="1">
         <v>1</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B44" s="2">
         <v>47.5</v>
@@ -3101,37 +2597,25 @@
       <c r="C44" s="3">
         <v>43292</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
       <c r="F44" s="3">
         <v>43292</v>
       </c>
-      <c r="G44" s="1">
-        <v>0</v>
-      </c>
-      <c r="H44" s="1">
-        <v>0</v>
-      </c>
-      <c r="I44" s="1">
-        <v>0</v>
-      </c>
       <c r="J44" s="1">
         <v>1</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2">
         <v>24</v>
@@ -3139,37 +2623,25 @@
       <c r="C45" s="3">
         <v>43292</v>
       </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
       <c r="F45" s="3">
         <v>43292</v>
       </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0</v>
-      </c>
       <c r="J45" s="1">
         <v>1</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" s="2">
         <v>5.23</v>
@@ -3177,40 +2649,28 @@
       <c r="C46" s="3">
         <v>43292</v>
       </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
       <c r="F46" s="3">
         <v>43292</v>
       </c>
-      <c r="G46" s="1">
-        <v>0</v>
-      </c>
-      <c r="H46" s="1">
-        <v>0</v>
-      </c>
-      <c r="I46" s="1">
-        <v>0</v>
-      </c>
       <c r="J46" s="1">
         <v>1</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="2">
         <v>11.5</v>
@@ -3218,40 +2678,28 @@
       <c r="C47" s="3">
         <v>43292</v>
       </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
       <c r="F47" s="3">
         <v>43292</v>
       </c>
-      <c r="G47" s="1">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1">
-        <v>0</v>
-      </c>
-      <c r="I47" s="1">
-        <v>0</v>
-      </c>
       <c r="J47" s="1">
         <v>1</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="2">
         <v>5.75</v>
@@ -3259,40 +2707,28 @@
       <c r="C48" s="3">
         <v>43292</v>
       </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
       <c r="F48" s="3">
         <v>43292</v>
       </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
       <c r="J48" s="1">
         <v>1</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="2">
         <v>10</v>
@@ -3300,40 +2736,28 @@
       <c r="C49" s="3">
         <v>43292</v>
       </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
       <c r="F49" s="3">
         <v>43292</v>
       </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49" s="1">
-        <v>0</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
       <c r="J49" s="1">
         <v>1</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50" s="2">
         <v>9</v>
@@ -3341,40 +2765,28 @@
       <c r="C50" s="3">
         <v>43292</v>
       </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
       <c r="F50" s="3">
         <v>43292</v>
       </c>
-      <c r="G50" s="1">
-        <v>0</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0</v>
-      </c>
-      <c r="I50" s="1">
-        <v>0</v>
-      </c>
       <c r="J50" s="1">
         <v>1</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51" s="2">
         <v>9</v>
@@ -3382,40 +2794,28 @@
       <c r="C51" s="3">
         <v>43292</v>
       </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
       <c r="F51" s="3">
         <v>43292</v>
       </c>
-      <c r="G51" s="1">
-        <v>0</v>
-      </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-      <c r="I51" s="1">
-        <v>0</v>
-      </c>
       <c r="J51" s="1">
         <v>1</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B52" s="2">
         <v>9</v>
@@ -3423,40 +2823,28 @@
       <c r="C52" s="3">
         <v>43292</v>
       </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
       <c r="F52" s="3">
         <v>43292</v>
       </c>
-      <c r="G52" s="1">
-        <v>0</v>
-      </c>
-      <c r="H52" s="1">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1">
-        <v>0</v>
-      </c>
       <c r="J52" s="1">
         <v>1</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2">
         <v>17.690000000000001</v>
@@ -3464,40 +2852,28 @@
       <c r="C53" s="3">
         <v>43292</v>
       </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
       <c r="F53" s="3">
         <v>43292</v>
       </c>
-      <c r="G53" s="1">
-        <v>0</v>
-      </c>
-      <c r="H53" s="1">
-        <v>0</v>
-      </c>
-      <c r="I53" s="1">
-        <v>0</v>
-      </c>
       <c r="J53" s="1">
         <v>1</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N53" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" s="2">
         <v>8.65</v>
@@ -3505,40 +2881,28 @@
       <c r="C54" s="3">
         <v>43292</v>
       </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
       <c r="F54" s="3">
         <v>43292</v>
       </c>
-      <c r="G54" s="1">
-        <v>0</v>
-      </c>
-      <c r="H54" s="1">
-        <v>0</v>
-      </c>
-      <c r="I54" s="1">
-        <v>0</v>
-      </c>
       <c r="J54" s="1">
         <v>1</v>
       </c>
       <c r="K54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="M54" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="N54" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B55" s="2">
         <v>6.87</v>
@@ -3546,40 +2910,28 @@
       <c r="C55" s="3">
         <v>43292</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
       <c r="F55" s="3">
         <v>43292</v>
       </c>
-      <c r="G55" s="1">
-        <v>0</v>
-      </c>
-      <c r="H55" s="1">
-        <v>0</v>
-      </c>
-      <c r="I55" s="1">
-        <v>0</v>
-      </c>
       <c r="J55" s="1">
         <v>1</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M55" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="N55" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B56" s="2">
         <v>8.7200000000000006</v>
@@ -3587,40 +2939,28 @@
       <c r="C56" s="3">
         <v>43292</v>
       </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
       <c r="F56" s="3">
         <v>43292</v>
       </c>
-      <c r="G56" s="1">
-        <v>0</v>
-      </c>
-      <c r="H56" s="1">
-        <v>0</v>
-      </c>
-      <c r="I56" s="1">
-        <v>0</v>
-      </c>
       <c r="J56" s="1">
         <v>1</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2">
         <v>12.22</v>
@@ -3628,40 +2968,28 @@
       <c r="C57" s="3">
         <v>43292</v>
       </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
       <c r="F57" s="3">
         <v>43292</v>
       </c>
-      <c r="G57" s="1">
-        <v>0</v>
-      </c>
-      <c r="H57" s="1">
-        <v>0</v>
-      </c>
-      <c r="I57" s="1">
-        <v>0</v>
-      </c>
       <c r="J57" s="1">
         <v>1</v>
       </c>
       <c r="K57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L57" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="M57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" s="2">
         <v>7.51</v>
@@ -3669,40 +2997,28 @@
       <c r="C58" s="3">
         <v>43292</v>
       </c>
-      <c r="E58" s="1">
-        <v>0</v>
-      </c>
       <c r="F58" s="3">
         <v>43292</v>
       </c>
-      <c r="G58" s="1">
-        <v>0</v>
-      </c>
-      <c r="H58" s="1">
-        <v>0</v>
-      </c>
-      <c r="I58" s="1">
-        <v>0</v>
-      </c>
       <c r="J58" s="1">
         <v>1</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="2">
         <v>8</v>
@@ -3710,40 +3026,28 @@
       <c r="C59" s="3">
         <v>43292</v>
       </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
       <c r="F59" s="3">
         <v>43292</v>
       </c>
-      <c r="G59" s="1">
-        <v>0</v>
-      </c>
-      <c r="H59" s="1">
-        <v>0</v>
-      </c>
-      <c r="I59" s="1">
-        <v>0</v>
-      </c>
       <c r="J59" s="1">
         <v>1</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M59" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N59" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B60" s="2">
         <v>26</v>
@@ -3751,37 +3055,25 @@
       <c r="C60" s="3">
         <v>43292</v>
       </c>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
       <c r="F60" s="3">
         <v>43292</v>
       </c>
-      <c r="G60" s="1">
-        <v>0</v>
-      </c>
-      <c r="H60" s="1">
-        <v>0</v>
-      </c>
-      <c r="I60" s="1">
-        <v>0</v>
-      </c>
       <c r="J60" s="1">
         <v>1</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2">
         <v>14.5</v>
@@ -3789,40 +3081,28 @@
       <c r="C61" s="3">
         <v>43292</v>
       </c>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
       <c r="F61" s="3">
         <v>43292</v>
       </c>
-      <c r="G61" s="1">
-        <v>0</v>
-      </c>
-      <c r="H61" s="1">
-        <v>0</v>
-      </c>
-      <c r="I61" s="1">
-        <v>0</v>
-      </c>
       <c r="J61" s="1">
         <v>1</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M61" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="N61" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" s="2">
         <v>18.5</v>
@@ -3830,40 +3110,28 @@
       <c r="C62" s="3">
         <v>43292</v>
       </c>
-      <c r="E62" s="1">
-        <v>0</v>
-      </c>
       <c r="F62" s="3">
         <v>43292</v>
       </c>
-      <c r="G62" s="1">
-        <v>0</v>
-      </c>
-      <c r="H62" s="1">
-        <v>0</v>
-      </c>
-      <c r="I62" s="1">
-        <v>0</v>
-      </c>
       <c r="J62" s="1">
         <v>1</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B63" s="2">
         <v>19.5</v>
@@ -3871,40 +3139,28 @@
       <c r="C63" s="3">
         <v>43292</v>
       </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
       <c r="F63" s="3">
         <v>43292</v>
       </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1">
-        <v>0</v>
-      </c>
-      <c r="I63" s="1">
-        <v>0</v>
-      </c>
       <c r="J63" s="1">
         <v>1</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64" s="2">
         <v>40</v>
@@ -3912,37 +3168,25 @@
       <c r="C64" s="3">
         <v>43292</v>
       </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
       <c r="F64" s="3">
         <v>43292</v>
       </c>
-      <c r="G64" s="1">
-        <v>0</v>
-      </c>
-      <c r="H64" s="1">
-        <v>0</v>
-      </c>
-      <c r="I64" s="1">
-        <v>0</v>
-      </c>
       <c r="J64" s="1">
         <v>1</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B65" s="2">
         <v>22.5</v>
@@ -3950,37 +3194,25 @@
       <c r="C65" s="3">
         <v>43292</v>
       </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
       <c r="F65" s="3">
         <v>43292</v>
       </c>
-      <c r="G65" s="1">
-        <v>0</v>
-      </c>
-      <c r="H65" s="1">
-        <v>0</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
       <c r="J65" s="1">
         <v>1</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B66" s="2">
         <v>61</v>
@@ -3988,37 +3220,25 @@
       <c r="C66" s="3">
         <v>43292</v>
       </c>
-      <c r="E66" s="1">
-        <v>0</v>
-      </c>
       <c r="F66" s="3">
         <v>43292</v>
       </c>
-      <c r="G66" s="1">
-        <v>0</v>
-      </c>
-      <c r="H66" s="1">
-        <v>0</v>
-      </c>
-      <c r="I66" s="1">
-        <v>0</v>
-      </c>
       <c r="J66" s="1">
         <v>1</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="2">
         <v>70.75</v>
@@ -4026,37 +3246,25 @@
       <c r="C67" s="3">
         <v>43292</v>
       </c>
-      <c r="E67" s="1">
-        <v>0</v>
-      </c>
       <c r="F67" s="3">
         <v>43292</v>
       </c>
-      <c r="G67" s="1">
-        <v>0</v>
-      </c>
-      <c r="H67" s="1">
-        <v>0</v>
-      </c>
-      <c r="I67" s="1">
-        <v>0</v>
-      </c>
       <c r="J67" s="1">
         <v>1</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B68" s="2">
         <v>20.75</v>
@@ -4064,37 +3272,25 @@
       <c r="C68" s="3">
         <v>43292</v>
       </c>
-      <c r="E68" s="1">
-        <v>0</v>
-      </c>
       <c r="F68" s="3">
         <v>43292</v>
       </c>
-      <c r="G68" s="1">
-        <v>0</v>
-      </c>
-      <c r="H68" s="1">
-        <v>0</v>
-      </c>
-      <c r="I68" s="1">
-        <v>0</v>
-      </c>
       <c r="J68" s="1">
         <v>1</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B69" s="2">
         <v>21.5</v>
@@ -4102,37 +3298,25 @@
       <c r="C69" s="3">
         <v>43292</v>
       </c>
-      <c r="E69" s="1">
-        <v>0</v>
-      </c>
       <c r="F69" s="3">
         <v>43292</v>
       </c>
-      <c r="G69" s="1">
-        <v>0</v>
-      </c>
-      <c r="H69" s="1">
-        <v>0</v>
-      </c>
-      <c r="I69" s="1">
-        <v>0</v>
-      </c>
       <c r="J69" s="1">
         <v>1</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B70" s="2">
         <v>14</v>
@@ -4140,40 +3324,28 @@
       <c r="C70" s="3">
         <v>43292</v>
       </c>
-      <c r="E70" s="1">
-        <v>0</v>
-      </c>
       <c r="F70" s="3">
         <v>43292</v>
       </c>
-      <c r="G70" s="1">
-        <v>0</v>
-      </c>
-      <c r="H70" s="1">
-        <v>0</v>
-      </c>
-      <c r="I70" s="1">
-        <v>0</v>
-      </c>
       <c r="J70" s="1">
         <v>1</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B71" s="2">
         <v>74.89</v>
@@ -4181,37 +3353,25 @@
       <c r="C71" s="3">
         <v>43292</v>
       </c>
-      <c r="E71" s="1">
-        <v>0</v>
-      </c>
       <c r="F71" s="3">
         <v>43292</v>
       </c>
-      <c r="G71" s="1">
-        <v>0</v>
-      </c>
-      <c r="H71" s="1">
-        <v>0</v>
-      </c>
-      <c r="I71" s="1">
-        <v>0</v>
-      </c>
       <c r="J71" s="1">
         <v>1</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B72" s="2">
         <v>61</v>
@@ -4219,40 +3379,28 @@
       <c r="C72" s="3">
         <v>43292</v>
       </c>
-      <c r="E72" s="1">
-        <v>0</v>
-      </c>
       <c r="F72" s="3">
         <v>43292</v>
       </c>
-      <c r="G72" s="1">
-        <v>0</v>
-      </c>
-      <c r="H72" s="1">
-        <v>0</v>
-      </c>
-      <c r="I72" s="1">
-        <v>0</v>
-      </c>
       <c r="J72" s="1">
         <v>1</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B73" s="2">
         <v>57.98</v>
@@ -4260,37 +3408,25 @@
       <c r="C73" s="3">
         <v>43292</v>
       </c>
-      <c r="E73" s="1">
-        <v>0</v>
-      </c>
       <c r="F73" s="3">
         <v>43292</v>
       </c>
-      <c r="G73" s="1">
-        <v>0</v>
-      </c>
-      <c r="H73" s="1">
-        <v>0</v>
-      </c>
-      <c r="I73" s="1">
-        <v>0</v>
-      </c>
       <c r="J73" s="1">
         <v>1</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B74" s="2">
         <v>20.5</v>
@@ -4298,40 +3434,28 @@
       <c r="C74" s="3">
         <v>43292</v>
       </c>
-      <c r="E74" s="1">
-        <v>0</v>
-      </c>
       <c r="F74" s="3">
         <v>43292</v>
       </c>
-      <c r="G74" s="1">
-        <v>0</v>
-      </c>
-      <c r="H74" s="1">
-        <v>0</v>
-      </c>
-      <c r="I74" s="1">
-        <v>0</v>
-      </c>
       <c r="J74" s="1">
         <v>1</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B75" s="2">
         <v>21</v>
@@ -4339,40 +3463,28 @@
       <c r="C75" s="3">
         <v>43292</v>
       </c>
-      <c r="E75" s="1">
-        <v>0</v>
-      </c>
       <c r="F75" s="3">
         <v>43292</v>
       </c>
-      <c r="G75" s="1">
-        <v>0</v>
-      </c>
-      <c r="H75" s="1">
-        <v>0</v>
-      </c>
-      <c r="I75" s="1">
-        <v>0</v>
-      </c>
       <c r="J75" s="1">
         <v>1</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" s="2">
         <v>13</v>
@@ -4380,40 +3492,28 @@
       <c r="C76" s="3">
         <v>43292</v>
       </c>
-      <c r="E76" s="1">
-        <v>0</v>
-      </c>
       <c r="F76" s="3">
         <v>43292</v>
       </c>
-      <c r="G76" s="1">
-        <v>0</v>
-      </c>
-      <c r="H76" s="1">
-        <v>0</v>
-      </c>
-      <c r="I76" s="1">
-        <v>0</v>
-      </c>
       <c r="J76" s="1">
         <v>1</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B77" s="2">
         <v>66</v>
@@ -4421,37 +3521,25 @@
       <c r="C77" s="3">
         <v>43292</v>
       </c>
-      <c r="E77" s="1">
-        <v>0</v>
-      </c>
       <c r="F77" s="3">
         <v>43292</v>
       </c>
-      <c r="G77" s="1">
-        <v>0</v>
-      </c>
-      <c r="H77" s="1">
-        <v>0</v>
-      </c>
-      <c r="I77" s="1">
-        <v>0</v>
-      </c>
       <c r="J77" s="1">
         <v>1</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="2">
         <v>10.35</v>
@@ -4459,40 +3547,28 @@
       <c r="C78" s="3">
         <v>43292</v>
       </c>
-      <c r="E78" s="1">
-        <v>0</v>
-      </c>
       <c r="F78" s="3">
         <v>43292</v>
       </c>
-      <c r="G78" s="1">
-        <v>0</v>
-      </c>
-      <c r="H78" s="1">
-        <v>0</v>
-      </c>
-      <c r="I78" s="1">
-        <v>0</v>
-      </c>
       <c r="J78" s="1">
         <v>1</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B79" s="2">
         <v>11.35</v>
@@ -4500,40 +3576,28 @@
       <c r="C79" s="3">
         <v>43292</v>
       </c>
-      <c r="E79" s="1">
-        <v>0</v>
-      </c>
       <c r="F79" s="3">
         <v>43292</v>
       </c>
-      <c r="G79" s="1">
-        <v>0</v>
-      </c>
-      <c r="H79" s="1">
-        <v>0</v>
-      </c>
-      <c r="I79" s="1">
-        <v>0</v>
-      </c>
       <c r="J79" s="1">
         <v>1</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B80" s="2">
         <v>36.549999999999997</v>
@@ -4541,37 +3605,25 @@
       <c r="C80" s="3">
         <v>43292</v>
       </c>
-      <c r="E80" s="1">
-        <v>0</v>
-      </c>
       <c r="F80" s="3">
         <v>43292</v>
       </c>
-      <c r="G80" s="1">
-        <v>0</v>
-      </c>
-      <c r="H80" s="1">
-        <v>0</v>
-      </c>
-      <c r="I80" s="1">
-        <v>0</v>
-      </c>
       <c r="J80" s="1">
         <v>1</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B81" s="2">
         <v>44.75</v>
@@ -4579,40 +3631,28 @@
       <c r="C81" s="3">
         <v>43292</v>
       </c>
-      <c r="E81" s="1">
-        <v>0</v>
-      </c>
       <c r="F81" s="3">
         <v>43292</v>
       </c>
-      <c r="G81" s="1">
-        <v>0</v>
-      </c>
-      <c r="H81" s="1">
-        <v>0</v>
-      </c>
-      <c r="I81" s="1">
-        <v>0</v>
-      </c>
       <c r="J81" s="1">
         <v>1</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M81" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="N81" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B82" s="2">
         <v>36.5</v>
@@ -4620,40 +3660,28 @@
       <c r="C82" s="3">
         <v>43292</v>
       </c>
-      <c r="E82" s="1">
-        <v>0</v>
-      </c>
       <c r="F82" s="3">
         <v>43292</v>
       </c>
-      <c r="G82" s="1">
-        <v>0</v>
-      </c>
-      <c r="H82" s="1">
-        <v>0</v>
-      </c>
-      <c r="I82" s="1">
-        <v>0</v>
-      </c>
       <c r="J82" s="1">
         <v>1</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B83" s="2">
         <v>22.9</v>
@@ -4661,40 +3689,28 @@
       <c r="C83" s="3">
         <v>43292</v>
       </c>
-      <c r="E83" s="1">
-        <v>0</v>
-      </c>
       <c r="F83" s="3">
         <v>43292</v>
       </c>
-      <c r="G83" s="1">
-        <v>0</v>
-      </c>
-      <c r="H83" s="1">
-        <v>0</v>
-      </c>
-      <c r="I83" s="1">
-        <v>0</v>
-      </c>
       <c r="J83" s="1">
         <v>1</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B84" s="2">
         <v>100</v>
@@ -4702,40 +3718,28 @@
       <c r="C84" s="3">
         <v>43292</v>
       </c>
-      <c r="E84" s="1">
-        <v>0</v>
-      </c>
       <c r="F84" s="3">
         <v>43292</v>
       </c>
-      <c r="G84" s="1">
-        <v>0</v>
-      </c>
-      <c r="H84" s="1">
-        <v>0</v>
-      </c>
-      <c r="I84" s="1">
-        <v>0</v>
-      </c>
       <c r="J84" s="1">
         <v>1</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="2">
         <v>42.5</v>
@@ -4743,40 +3747,28 @@
       <c r="C85" s="3">
         <v>43292</v>
       </c>
-      <c r="E85" s="1">
-        <v>0</v>
-      </c>
       <c r="F85" s="3">
         <v>43292</v>
       </c>
-      <c r="G85" s="1">
-        <v>0</v>
-      </c>
-      <c r="H85" s="1">
-        <v>0</v>
-      </c>
-      <c r="I85" s="1">
-        <v>0</v>
-      </c>
       <c r="J85" s="1">
         <v>1</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B86" s="2">
         <v>29</v>
@@ -4784,40 +3776,28 @@
       <c r="C86" s="3">
         <v>43292</v>
       </c>
-      <c r="E86" s="1">
-        <v>0</v>
-      </c>
       <c r="F86" s="3">
         <v>43292</v>
       </c>
-      <c r="G86" s="1">
-        <v>0</v>
-      </c>
-      <c r="H86" s="1">
-        <v>0</v>
-      </c>
-      <c r="I86" s="1">
-        <v>0</v>
-      </c>
       <c r="J86" s="1">
         <v>1</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B87" s="2">
         <v>21.5</v>
@@ -4825,40 +3805,28 @@
       <c r="C87" s="3">
         <v>43292</v>
       </c>
-      <c r="E87" s="1">
-        <v>0</v>
-      </c>
       <c r="F87" s="3">
         <v>43292</v>
       </c>
-      <c r="G87" s="1">
-        <v>0</v>
-      </c>
-      <c r="H87" s="1">
-        <v>0</v>
-      </c>
-      <c r="I87" s="1">
-        <v>0</v>
-      </c>
       <c r="J87" s="1">
         <v>1</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B88" s="2">
         <v>26</v>
@@ -4866,37 +3834,25 @@
       <c r="C88" s="3">
         <v>43292</v>
       </c>
-      <c r="E88" s="1">
-        <v>0</v>
-      </c>
       <c r="F88" s="3">
         <v>43292</v>
       </c>
-      <c r="G88" s="1">
-        <v>0</v>
-      </c>
-      <c r="H88" s="1">
-        <v>0</v>
-      </c>
-      <c r="I88" s="1">
-        <v>0</v>
-      </c>
       <c r="J88" s="1">
         <v>1</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B89" s="2">
         <v>96.25</v>
@@ -4904,37 +3860,25 @@
       <c r="C89" s="3">
         <v>43292</v>
       </c>
-      <c r="E89" s="1">
-        <v>0</v>
-      </c>
       <c r="F89" s="3">
         <v>43292</v>
       </c>
-      <c r="G89" s="1">
-        <v>0</v>
-      </c>
-      <c r="H89" s="1">
-        <v>0</v>
-      </c>
-      <c r="I89" s="1">
-        <v>0</v>
-      </c>
       <c r="J89" s="1">
         <v>1</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B90" s="2">
         <v>16.5</v>
@@ -4942,37 +3886,25 @@
       <c r="C90" s="3">
         <v>43292</v>
       </c>
-      <c r="E90" s="1">
-        <v>0</v>
-      </c>
       <c r="F90" s="3">
         <v>43292</v>
       </c>
-      <c r="G90" s="1">
-        <v>0</v>
-      </c>
-      <c r="H90" s="1">
-        <v>0</v>
-      </c>
-      <c r="I90" s="1">
-        <v>0</v>
-      </c>
       <c r="J90" s="1">
         <v>1</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B91" s="2">
         <v>9.1999999999999993</v>
@@ -4980,37 +3912,25 @@
       <c r="C91" s="3">
         <v>43292</v>
       </c>
-      <c r="E91" s="1">
-        <v>0</v>
-      </c>
       <c r="F91" s="3">
         <v>43292</v>
       </c>
-      <c r="G91" s="1">
-        <v>0</v>
-      </c>
-      <c r="H91" s="1">
-        <v>0</v>
-      </c>
-      <c r="I91" s="1">
-        <v>0</v>
-      </c>
       <c r="J91" s="1">
         <v>1</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B92" s="2">
         <v>21</v>
@@ -5018,37 +3938,25 @@
       <c r="C92" s="3">
         <v>43292</v>
       </c>
-      <c r="E92" s="1">
-        <v>0</v>
-      </c>
       <c r="F92" s="3">
         <v>43292</v>
       </c>
-      <c r="G92" s="1">
-        <v>0</v>
-      </c>
-      <c r="H92" s="1">
-        <v>0</v>
-      </c>
-      <c r="I92" s="1">
-        <v>0</v>
-      </c>
       <c r="J92" s="1">
         <v>1</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B93" s="2">
         <v>20.5</v>
@@ -5056,37 +3964,25 @@
       <c r="C93" s="3">
         <v>43292</v>
       </c>
-      <c r="E93" s="1">
-        <v>0</v>
-      </c>
       <c r="F93" s="3">
         <v>43292</v>
       </c>
-      <c r="G93" s="1">
-        <v>0</v>
-      </c>
-      <c r="H93" s="1">
-        <v>0</v>
-      </c>
-      <c r="I93" s="1">
-        <v>0</v>
-      </c>
       <c r="J93" s="1">
         <v>1</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B94" s="2">
         <v>20</v>
@@ -5094,37 +3990,25 @@
       <c r="C94" s="3">
         <v>43292</v>
       </c>
-      <c r="E94" s="1">
-        <v>0</v>
-      </c>
       <c r="F94" s="3">
         <v>43292</v>
       </c>
-      <c r="G94" s="1">
-        <v>0</v>
-      </c>
-      <c r="H94" s="1">
-        <v>0</v>
-      </c>
-      <c r="I94" s="1">
-        <v>0</v>
-      </c>
       <c r="J94" s="1">
         <v>1</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B95" s="2">
         <v>1</v>
@@ -5132,37 +4016,25 @@
       <c r="C95" s="3">
         <v>43292</v>
       </c>
-      <c r="E95" s="1">
-        <v>0</v>
-      </c>
       <c r="F95" s="3">
         <v>43292</v>
       </c>
-      <c r="G95" s="1">
-        <v>0</v>
-      </c>
-      <c r="H95" s="1">
-        <v>0</v>
-      </c>
-      <c r="I95" s="1">
-        <v>0</v>
-      </c>
       <c r="J95" s="1">
         <v>1</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B96" s="2">
         <v>38.5</v>
@@ -5170,37 +4042,25 @@
       <c r="C96" s="3">
         <v>43292</v>
       </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
       <c r="F96" s="3">
         <v>43292</v>
       </c>
-      <c r="G96" s="1">
-        <v>0</v>
-      </c>
-      <c r="H96" s="1">
-        <v>0</v>
-      </c>
-      <c r="I96" s="1">
-        <v>0</v>
-      </c>
       <c r="J96" s="1">
         <v>1</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B97" s="2">
         <v>55</v>
@@ -5208,37 +4068,25 @@
       <c r="C97" s="3">
         <v>43292</v>
       </c>
-      <c r="E97" s="1">
-        <v>0</v>
-      </c>
       <c r="F97" s="3">
         <v>43292</v>
       </c>
-      <c r="G97" s="1">
-        <v>0</v>
-      </c>
-      <c r="H97" s="1">
-        <v>0</v>
-      </c>
-      <c r="I97" s="1">
-        <v>0</v>
-      </c>
       <c r="J97" s="1">
         <v>1</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" s="2">
         <v>31.25</v>
@@ -5246,37 +4094,25 @@
       <c r="C98" s="3">
         <v>43292</v>
       </c>
-      <c r="E98" s="1">
-        <v>0</v>
-      </c>
       <c r="F98" s="3">
         <v>43292</v>
       </c>
-      <c r="G98" s="1">
-        <v>0</v>
-      </c>
-      <c r="H98" s="1">
-        <v>0</v>
-      </c>
-      <c r="I98" s="1">
-        <v>0</v>
-      </c>
       <c r="J98" s="1">
         <v>1</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B99" s="2">
         <v>50</v>
@@ -5284,37 +4120,25 @@
       <c r="C99" s="3">
         <v>43292</v>
       </c>
-      <c r="E99" s="1">
-        <v>0</v>
-      </c>
       <c r="F99" s="3">
         <v>43292</v>
       </c>
-      <c r="G99" s="1">
-        <v>0</v>
-      </c>
-      <c r="H99" s="1">
-        <v>0</v>
-      </c>
-      <c r="I99" s="1">
-        <v>0</v>
-      </c>
       <c r="J99" s="1">
         <v>1</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B100" s="2">
         <v>35</v>
@@ -5322,32 +4146,20 @@
       <c r="C100" s="3">
         <v>43292</v>
       </c>
-      <c r="E100" s="1">
-        <v>0</v>
-      </c>
       <c r="F100" s="3">
         <v>43292</v>
       </c>
-      <c r="G100" s="1">
-        <v>0</v>
-      </c>
-      <c r="H100" s="1">
-        <v>0</v>
-      </c>
-      <c r="I100" s="1">
-        <v>0</v>
-      </c>
       <c r="J100" s="1">
         <v>1</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>